<commit_message>
Bailey tech book finish
</commit_message>
<xml_diff>
--- a/Excel/Bailey/Bailey — техничка.xlsx
+++ b/Excel/Bailey/Bailey — техничка.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BUH\Documents\HatsAndCaps\Excel\Bailey\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81FFB49E-3A6D-4D56-9D4D-83E748B98CF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8CF3B5B-DF19-4523-B4DE-BD48B06C6C2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3DF93E06-745E-43BB-B362-39D65D7A1090}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3915" uniqueCount="610">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4091" uniqueCount="610">
   <si>
     <t>Артикул на этикетке</t>
   </si>
@@ -9884,6 +9884,551 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>81642</xdr:colOff>
+      <xdr:row>156</xdr:row>
+      <xdr:rowOff>330759</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>1815473</xdr:colOff>
+      <xdr:row>156</xdr:row>
+      <xdr:rowOff>1529804</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="205" name="Рисунок 204">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B9352874-3733-4E19-9A42-A50C4E324C16}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId155"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4313463" y="229202902"/>
+          <a:ext cx="1733831" cy="1199045"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>68033</xdr:colOff>
+      <xdr:row>157</xdr:row>
+      <xdr:rowOff>266910</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>1842900</xdr:colOff>
+      <xdr:row>157</xdr:row>
+      <xdr:rowOff>1514282</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="206" name="Рисунок 205">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{67FFF8E6-AE9D-43F5-A250-652B2A5E650B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId156"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4299854" y="230907981"/>
+          <a:ext cx="1774867" cy="1247372"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>136071</xdr:colOff>
+      <xdr:row>158</xdr:row>
+      <xdr:rowOff>284703</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>1839123</xdr:colOff>
+      <xdr:row>158</xdr:row>
+      <xdr:rowOff>1494292</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="207" name="Рисунок 206">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{46B51E9B-C1DF-414B-B7C1-68F4D5C434A5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId157"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4367892" y="232694703"/>
+          <a:ext cx="1703052" cy="1209589"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>68035</xdr:colOff>
+      <xdr:row>159</xdr:row>
+      <xdr:rowOff>275284</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>1842901</xdr:colOff>
+      <xdr:row>159</xdr:row>
+      <xdr:rowOff>1566096</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="208" name="Рисунок 207">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C4C81AC8-05E7-4D3A-93F0-AD9B5711B008}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId158"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4299856" y="234454213"/>
+          <a:ext cx="1774866" cy="1290812"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>40819</xdr:colOff>
+      <xdr:row>160</xdr:row>
+      <xdr:rowOff>347506</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>1824805</xdr:colOff>
+      <xdr:row>160</xdr:row>
+      <xdr:rowOff>1527331</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="209" name="Рисунок 208">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{52B66C4D-EA7D-46D2-A565-3BF9AE6E2D1C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId159"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4272640" y="236295363"/>
+          <a:ext cx="1783986" cy="1179825"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>54426</xdr:colOff>
+      <xdr:row>161</xdr:row>
+      <xdr:rowOff>310873</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>1891393</xdr:colOff>
+      <xdr:row>161</xdr:row>
+      <xdr:rowOff>1583033</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="210" name="Рисунок 209">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F98FB93C-5E57-4A85-90DC-631A8515D136}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId160"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4286247" y="238027659"/>
+          <a:ext cx="1836967" cy="1272160"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>27214</xdr:colOff>
+      <xdr:row>155</xdr:row>
+      <xdr:rowOff>244928</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>1855212</xdr:colOff>
+      <xdr:row>155</xdr:row>
+      <xdr:rowOff>1537607</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="211" name="Рисунок 210">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A13E9918-1AEE-4C57-8706-490AC4EB41CB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId161"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4259035" y="227348142"/>
+          <a:ext cx="1827998" cy="1292679"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>122463</xdr:colOff>
+      <xdr:row>165</xdr:row>
+      <xdr:rowOff>422868</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>1887691</xdr:colOff>
+      <xdr:row>165</xdr:row>
+      <xdr:rowOff>1520619</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="212" name="Рисунок 211">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{168C1B50-00AC-4847-A9C2-C06ACF110348}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId162"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4354284" y="245215368"/>
+          <a:ext cx="1765228" cy="1097751"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>95248</xdr:colOff>
+      <xdr:row>164</xdr:row>
+      <xdr:rowOff>405076</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>1907467</xdr:colOff>
+      <xdr:row>164</xdr:row>
+      <xdr:rowOff>1482308</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="213" name="Рисунок 212">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7DBFD9DA-B505-4FCD-B5C6-3CC08A0EB2D7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId163"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4327069" y="243428647"/>
+          <a:ext cx="1812219" cy="1077232"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>1142998</xdr:colOff>
+      <xdr:row>164</xdr:row>
+      <xdr:rowOff>1044726</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>1748299</xdr:colOff>
+      <xdr:row>164</xdr:row>
+      <xdr:rowOff>1508361</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="214" name="Рисунок 213">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BD62AF2E-173E-4DF4-AE9F-6B0082C4C6E7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId164">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="5374819" y="244068297"/>
+          <a:ext cx="605301" cy="463635"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>145491</xdr:colOff>
+      <xdr:row>163</xdr:row>
+      <xdr:rowOff>352740</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>18733</xdr:colOff>
+      <xdr:row>163</xdr:row>
+      <xdr:rowOff>1523884</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="215" name="Рисунок 214">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{16F413FE-0B60-41C5-AC8F-6E23263BFD8D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId165"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4377312" y="241607383"/>
+          <a:ext cx="1791850" cy="1171144"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>101529</xdr:colOff>
+      <xdr:row>162</xdr:row>
+      <xdr:rowOff>363206</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>1914991</xdr:colOff>
+      <xdr:row>162</xdr:row>
+      <xdr:rowOff>1545399</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="216" name="Рисунок 215">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A4B4CF61-1CBF-4203-9213-3A846E6BDD5E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId166"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4333350" y="239848920"/>
+          <a:ext cx="1813462" cy="1182193"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -13552,15 +14097,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>68036</xdr:colOff>
+      <xdr:colOff>68037</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>95251</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>2367643</xdr:colOff>
+      <xdr:colOff>2074225</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>1685563</xdr:rowOff>
+      <xdr:rowOff>1482647</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -13583,8 +14128,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4306661" y="2695576"/>
-          <a:ext cx="2299607" cy="1590312"/>
+          <a:off x="4317652" y="2703636"/>
+          <a:ext cx="2006188" cy="1387396"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -13602,9 +14147,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>2408463</xdr:colOff>
+      <xdr:colOff>2108099</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>1681624</xdr:rowOff>
+      <xdr:rowOff>1470529</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -13627,8 +14172,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4293053" y="4399189"/>
-          <a:ext cx="2354035" cy="1654410"/>
+          <a:off x="4304043" y="4408714"/>
+          <a:ext cx="2053671" cy="1443315"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -13646,9 +14191,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>2381251</xdr:colOff>
+      <xdr:colOff>2093040</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>1645120</xdr:rowOff>
+      <xdr:rowOff>1440419</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -13671,8 +14216,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4361090" y="6184447"/>
-          <a:ext cx="2258786" cy="1604298"/>
+          <a:off x="4372080" y="6195437"/>
+          <a:ext cx="1970575" cy="1399597"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -13690,9 +14235,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>2408463</xdr:colOff>
+      <xdr:colOff>2108100</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>1739240</xdr:rowOff>
+      <xdr:rowOff>1520794</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -13715,8 +14260,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4293054" y="7942490"/>
-          <a:ext cx="2354034" cy="1712025"/>
+          <a:off x="4304044" y="7954946"/>
+          <a:ext cx="2053671" cy="1493579"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -13734,9 +14279,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>2393342</xdr:colOff>
+      <xdr:colOff>2091436</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>1660071</xdr:rowOff>
+      <xdr:rowOff>1460408</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -13759,8 +14304,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4265839" y="9782176"/>
-          <a:ext cx="2366128" cy="1564820"/>
+          <a:off x="4276829" y="9796097"/>
+          <a:ext cx="2064222" cy="1365157"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -13778,9 +14323,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>2550971</xdr:colOff>
+      <xdr:colOff>2230689</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>1741716</xdr:rowOff>
+      <xdr:rowOff>1526427</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -13803,8 +14348,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4279446" y="11513005"/>
-          <a:ext cx="2510150" cy="1687286"/>
+          <a:off x="4290436" y="11528392"/>
+          <a:ext cx="2189868" cy="1471997"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -13816,15 +14361,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>13608</xdr:colOff>
+      <xdr:colOff>13609</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>13607</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>2438111</xdr:colOff>
+      <xdr:colOff>2128757</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>1728108</xdr:rowOff>
+      <xdr:rowOff>1509346</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -13847,8 +14392,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4252233" y="842282"/>
-          <a:ext cx="2424503" cy="1714501"/>
+          <a:off x="4263224" y="848876"/>
+          <a:ext cx="2115148" cy="1495739"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -13866,9 +14411,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>2450108</xdr:colOff>
+      <xdr:colOff>2151376</xdr:colOff>
       <xdr:row>11</xdr:row>
-      <xdr:rowOff>1605644</xdr:rowOff>
+      <xdr:rowOff>1419870</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -13891,8 +14436,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4347483" y="18694854"/>
-          <a:ext cx="2341250" cy="1455965"/>
+          <a:off x="4358473" y="18716102"/>
+          <a:ext cx="2042518" cy="1270191"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -13910,9 +14455,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>2485219</xdr:colOff>
+      <xdr:colOff>2178534</xdr:colOff>
       <xdr:row>10</xdr:row>
-      <xdr:rowOff>1564823</xdr:rowOff>
+      <xdr:rowOff>1382521</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -13935,8 +14480,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4320268" y="16909597"/>
-          <a:ext cx="2403576" cy="1428751"/>
+          <a:off x="4331258" y="16929380"/>
+          <a:ext cx="2096891" cy="1246449"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -13954,9 +14499,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>2490107</xdr:colOff>
+      <xdr:colOff>2387671</xdr:colOff>
       <xdr:row>10</xdr:row>
-      <xdr:rowOff>1635578</xdr:rowOff>
+      <xdr:rowOff>1557116</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -13986,8 +14531,8 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="5925911" y="17794176"/>
-          <a:ext cx="802821" cy="614927"/>
+          <a:off x="5936901" y="17813959"/>
+          <a:ext cx="700385" cy="536465"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14015,9 +14560,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>2508446</xdr:colOff>
+      <xdr:colOff>2205208</xdr:colOff>
       <xdr:row>9</xdr:row>
-      <xdr:rowOff>1641232</xdr:rowOff>
+      <xdr:rowOff>1443037</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14040,8 +14585,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4370510" y="15089799"/>
-          <a:ext cx="2376561" cy="1553308"/>
+          <a:off x="4381500" y="15108116"/>
+          <a:ext cx="2073323" cy="1355113"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14059,9 +14604,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>2493146</xdr:colOff>
+      <xdr:colOff>2186252</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>1670538</xdr:rowOff>
+      <xdr:rowOff>1470474</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -14084,8 +14629,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4326548" y="13332802"/>
-          <a:ext cx="2405223" cy="1567961"/>
+          <a:off x="4337538" y="13349654"/>
+          <a:ext cx="2098329" cy="1367897"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14397,11 +14942,11 @@
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
-  <dimension ref="A1:AM262"/>
+  <dimension ref="A1:AN262"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A153" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F156" sqref="F156"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M7" sqref="M7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="78" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -14412,7 +14957,7 @@
     <col min="5" max="5" width="9" style="26"/>
     <col min="6" max="6" width="9" style="23"/>
     <col min="7" max="7" width="9" style="26"/>
-    <col min="8" max="8" width="27.42578125" style="26" customWidth="1"/>
+    <col min="8" max="8" width="28.85546875" style="26" customWidth="1"/>
     <col min="9" max="9" width="9" style="26"/>
     <col min="10" max="10" width="9" style="30"/>
     <col min="11" max="11" width="9" style="26"/>
@@ -29061,27 +29606,1044 @@
         <v>6</v>
       </c>
     </row>
-    <row r="156" spans="1:39" ht="140.1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="157" spans="1:39" ht="140.1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="158" spans="1:39" ht="140.1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="159" spans="1:39" ht="140.1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="160" spans="1:39" ht="140.1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="161" ht="140.1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="162" ht="140.1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="163" ht="140.1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="164" ht="140.1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="165" ht="140.1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="166" ht="140.1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="167" ht="140.1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="168" ht="140.1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="169" ht="140.1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="170" ht="140.1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="171" ht="140.1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="172" ht="140.1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="173" ht="140.1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="174" ht="140.1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="175" ht="140.1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="176" ht="140.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="156" spans="1:39" ht="140.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A156" s="11" t="s">
+        <v>565</v>
+      </c>
+      <c r="B156" s="12" t="s">
+        <v>566</v>
+      </c>
+      <c r="C156" s="13" t="s">
+        <v>567</v>
+      </c>
+      <c r="D156" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="E156" s="13" t="s">
+        <v>568</v>
+      </c>
+      <c r="F156" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="G156" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="H156" s="46"/>
+      <c r="I156" s="15" t="s">
+        <v>421</v>
+      </c>
+      <c r="J156" s="16" t="s">
+        <v>569</v>
+      </c>
+      <c r="K156" s="44" t="s">
+        <v>570</v>
+      </c>
+      <c r="L156" s="18" t="s">
+        <v>571</v>
+      </c>
+      <c r="M156" s="19"/>
+      <c r="N156" s="12" t="s">
+        <v>424</v>
+      </c>
+      <c r="O156" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="P156" s="12"/>
+      <c r="Q156" s="12"/>
+      <c r="R156" s="12"/>
+      <c r="S156" s="12"/>
+      <c r="T156" s="12"/>
+      <c r="U156" s="12">
+        <v>1</v>
+      </c>
+      <c r="V156" s="12"/>
+      <c r="W156" s="12"/>
+      <c r="X156" s="12"/>
+      <c r="Y156" s="12"/>
+      <c r="Z156" s="12"/>
+      <c r="AA156" s="12"/>
+      <c r="AB156" s="12"/>
+      <c r="AC156" s="12"/>
+      <c r="AD156" s="15">
+        <v>1</v>
+      </c>
+      <c r="AE156" s="17" t="s">
+        <v>77</v>
+      </c>
+      <c r="AF156" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="AG156" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="AH156" s="20">
+        <v>0.1</v>
+      </c>
+      <c r="AI156" s="13">
+        <v>0.15000000000000002</v>
+      </c>
+      <c r="AJ156" s="13">
+        <v>0.1</v>
+      </c>
+      <c r="AK156" s="13">
+        <v>0.15000000000000002</v>
+      </c>
+      <c r="AL156" s="39">
+        <v>6</v>
+      </c>
+      <c r="AM156" s="40">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="157" spans="1:39" ht="140.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A157" s="11" t="s">
+        <v>572</v>
+      </c>
+      <c r="B157" s="12" t="s">
+        <v>573</v>
+      </c>
+      <c r="C157" s="12" t="s">
+        <v>574</v>
+      </c>
+      <c r="D157" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="E157" s="12" t="s">
+        <v>568</v>
+      </c>
+      <c r="F157" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="G157" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="H157" s="12"/>
+      <c r="I157" s="15" t="s">
+        <v>421</v>
+      </c>
+      <c r="J157" s="24" t="s">
+        <v>433</v>
+      </c>
+      <c r="K157" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="L157" s="45" t="s">
+        <v>469</v>
+      </c>
+      <c r="M157" s="19"/>
+      <c r="N157" s="12" t="s">
+        <v>424</v>
+      </c>
+      <c r="O157" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="P157" s="12"/>
+      <c r="Q157" s="12"/>
+      <c r="R157" s="12"/>
+      <c r="S157" s="12">
+        <v>1</v>
+      </c>
+      <c r="T157" s="12"/>
+      <c r="U157" s="12"/>
+      <c r="V157" s="12"/>
+      <c r="W157" s="12"/>
+      <c r="X157" s="12"/>
+      <c r="Y157" s="12"/>
+      <c r="Z157" s="12"/>
+      <c r="AA157" s="12"/>
+      <c r="AB157" s="12"/>
+      <c r="AC157" s="12"/>
+      <c r="AD157" s="15">
+        <v>1</v>
+      </c>
+      <c r="AE157" s="44" t="s">
+        <v>77</v>
+      </c>
+      <c r="AF157" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="AG157" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="AH157" s="20">
+        <v>0.1</v>
+      </c>
+      <c r="AI157" s="13">
+        <v>0.15000000000000002</v>
+      </c>
+      <c r="AJ157" s="13">
+        <v>0.1</v>
+      </c>
+      <c r="AK157" s="13">
+        <v>0.15000000000000002</v>
+      </c>
+      <c r="AL157" s="39">
+        <v>6</v>
+      </c>
+      <c r="AM157" s="40">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="158" spans="1:39" ht="140.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A158" s="11" t="s">
+        <v>575</v>
+      </c>
+      <c r="B158" s="12" t="s">
+        <v>576</v>
+      </c>
+      <c r="C158" s="12" t="s">
+        <v>577</v>
+      </c>
+      <c r="D158" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="E158" s="12" t="s">
+        <v>568</v>
+      </c>
+      <c r="F158" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="G158" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="H158" s="12"/>
+      <c r="I158" s="15" t="s">
+        <v>421</v>
+      </c>
+      <c r="J158" s="24" t="s">
+        <v>578</v>
+      </c>
+      <c r="K158" s="12" t="s">
+        <v>570</v>
+      </c>
+      <c r="L158" s="45" t="s">
+        <v>469</v>
+      </c>
+      <c r="M158" s="19"/>
+      <c r="N158" s="12" t="s">
+        <v>424</v>
+      </c>
+      <c r="O158" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="P158" s="12"/>
+      <c r="Q158" s="12"/>
+      <c r="R158" s="12"/>
+      <c r="S158" s="12"/>
+      <c r="T158" s="12"/>
+      <c r="U158" s="12"/>
+      <c r="V158" s="12"/>
+      <c r="W158" s="12"/>
+      <c r="X158" s="12"/>
+      <c r="Y158" s="12"/>
+      <c r="Z158" s="12">
+        <v>1</v>
+      </c>
+      <c r="AA158" s="12"/>
+      <c r="AB158" s="12"/>
+      <c r="AC158" s="12"/>
+      <c r="AD158" s="15">
+        <v>1</v>
+      </c>
+      <c r="AE158" s="44" t="s">
+        <v>77</v>
+      </c>
+      <c r="AF158" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="AG158" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="AH158" s="20">
+        <v>0.1</v>
+      </c>
+      <c r="AI158" s="13">
+        <v>0.15000000000000002</v>
+      </c>
+      <c r="AJ158" s="13">
+        <v>0.1</v>
+      </c>
+      <c r="AK158" s="13">
+        <v>0.15000000000000002</v>
+      </c>
+      <c r="AL158" s="39">
+        <v>6</v>
+      </c>
+      <c r="AM158" s="40">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="159" spans="1:39" ht="140.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A159" s="11" t="s">
+        <v>579</v>
+      </c>
+      <c r="B159" s="12" t="s">
+        <v>580</v>
+      </c>
+      <c r="C159" s="12" t="s">
+        <v>581</v>
+      </c>
+      <c r="D159" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="E159" s="12" t="s">
+        <v>568</v>
+      </c>
+      <c r="F159" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="G159" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="H159" s="12"/>
+      <c r="I159" s="15" t="s">
+        <v>421</v>
+      </c>
+      <c r="J159" s="24" t="s">
+        <v>582</v>
+      </c>
+      <c r="K159" s="12" t="s">
+        <v>142</v>
+      </c>
+      <c r="L159" s="45" t="s">
+        <v>469</v>
+      </c>
+      <c r="M159" s="19"/>
+      <c r="N159" s="12" t="s">
+        <v>424</v>
+      </c>
+      <c r="O159" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="P159" s="12"/>
+      <c r="Q159" s="12"/>
+      <c r="R159" s="12"/>
+      <c r="S159" s="12"/>
+      <c r="T159" s="12"/>
+      <c r="U159" s="12">
+        <v>1</v>
+      </c>
+      <c r="V159" s="12"/>
+      <c r="W159" s="12"/>
+      <c r="X159" s="12"/>
+      <c r="Y159" s="12"/>
+      <c r="Z159" s="12"/>
+      <c r="AA159" s="12"/>
+      <c r="AB159" s="12"/>
+      <c r="AC159" s="12"/>
+      <c r="AD159" s="15">
+        <v>1</v>
+      </c>
+      <c r="AE159" s="44" t="s">
+        <v>77</v>
+      </c>
+      <c r="AF159" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="AG159" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="AH159" s="20">
+        <v>0.1</v>
+      </c>
+      <c r="AI159" s="13">
+        <v>0.15000000000000002</v>
+      </c>
+      <c r="AJ159" s="13">
+        <v>0.1</v>
+      </c>
+      <c r="AK159" s="13">
+        <v>0.15000000000000002</v>
+      </c>
+      <c r="AL159" s="39">
+        <v>6</v>
+      </c>
+      <c r="AM159" s="40">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="160" spans="1:39" ht="140.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A160" s="11" t="s">
+        <v>583</v>
+      </c>
+      <c r="B160" s="12" t="s">
+        <v>584</v>
+      </c>
+      <c r="C160" s="12" t="s">
+        <v>585</v>
+      </c>
+      <c r="D160" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="E160" s="12" t="s">
+        <v>568</v>
+      </c>
+      <c r="F160" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="G160" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="H160" s="12"/>
+      <c r="I160" s="15" t="s">
+        <v>421</v>
+      </c>
+      <c r="J160" s="24" t="s">
+        <v>433</v>
+      </c>
+      <c r="K160" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="L160" s="45" t="s">
+        <v>469</v>
+      </c>
+      <c r="M160" s="19"/>
+      <c r="N160" s="12" t="s">
+        <v>424</v>
+      </c>
+      <c r="O160" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="P160" s="12"/>
+      <c r="Q160" s="12"/>
+      <c r="R160" s="12"/>
+      <c r="S160" s="12"/>
+      <c r="T160" s="12"/>
+      <c r="U160" s="12"/>
+      <c r="V160" s="12"/>
+      <c r="W160" s="12">
+        <v>1</v>
+      </c>
+      <c r="X160" s="12"/>
+      <c r="Y160" s="12"/>
+      <c r="Z160" s="12"/>
+      <c r="AA160" s="12"/>
+      <c r="AB160" s="12"/>
+      <c r="AC160" s="12"/>
+      <c r="AD160" s="15">
+        <v>1</v>
+      </c>
+      <c r="AE160" s="44" t="s">
+        <v>77</v>
+      </c>
+      <c r="AF160" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="AG160" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="AH160" s="20">
+        <v>0.1</v>
+      </c>
+      <c r="AI160" s="13">
+        <v>0.15000000000000002</v>
+      </c>
+      <c r="AJ160" s="13">
+        <v>0.1</v>
+      </c>
+      <c r="AK160" s="13">
+        <v>0.15000000000000002</v>
+      </c>
+      <c r="AL160" s="39">
+        <v>6</v>
+      </c>
+      <c r="AM160" s="40">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="161" spans="1:40" ht="140.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A161" s="11" t="s">
+        <v>586</v>
+      </c>
+      <c r="B161" s="12" t="s">
+        <v>587</v>
+      </c>
+      <c r="C161" s="12" t="s">
+        <v>588</v>
+      </c>
+      <c r="D161" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="E161" s="12" t="s">
+        <v>568</v>
+      </c>
+      <c r="F161" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="G161" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="H161" s="12"/>
+      <c r="I161" s="15" t="s">
+        <v>421</v>
+      </c>
+      <c r="J161" s="24" t="s">
+        <v>433</v>
+      </c>
+      <c r="K161" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="L161" s="45" t="s">
+        <v>469</v>
+      </c>
+      <c r="M161" s="19"/>
+      <c r="N161" s="12" t="s">
+        <v>424</v>
+      </c>
+      <c r="O161" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="P161" s="12"/>
+      <c r="Q161" s="12"/>
+      <c r="R161" s="12"/>
+      <c r="S161" s="12"/>
+      <c r="T161" s="12"/>
+      <c r="U161" s="12">
+        <v>1</v>
+      </c>
+      <c r="V161" s="12"/>
+      <c r="W161" s="12"/>
+      <c r="X161" s="12"/>
+      <c r="Y161" s="12"/>
+      <c r="Z161" s="12"/>
+      <c r="AA161" s="12"/>
+      <c r="AB161" s="12"/>
+      <c r="AC161" s="12"/>
+      <c r="AD161" s="15">
+        <v>1</v>
+      </c>
+      <c r="AE161" s="44" t="s">
+        <v>77</v>
+      </c>
+      <c r="AF161" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="AG161" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="AH161" s="20">
+        <v>0.1</v>
+      </c>
+      <c r="AI161" s="13">
+        <v>0.15000000000000002</v>
+      </c>
+      <c r="AJ161" s="13">
+        <v>0.1</v>
+      </c>
+      <c r="AK161" s="13">
+        <v>0.15000000000000002</v>
+      </c>
+      <c r="AL161" s="39">
+        <v>6</v>
+      </c>
+      <c r="AM161" s="40">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="162" spans="1:40" ht="140.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A162" s="11" t="s">
+        <v>589</v>
+      </c>
+      <c r="B162" s="12" t="s">
+        <v>590</v>
+      </c>
+      <c r="C162" s="12" t="s">
+        <v>591</v>
+      </c>
+      <c r="D162" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="E162" s="12" t="s">
+        <v>568</v>
+      </c>
+      <c r="F162" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="G162" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="H162" s="12"/>
+      <c r="I162" s="15" t="s">
+        <v>421</v>
+      </c>
+      <c r="J162" s="24" t="s">
+        <v>592</v>
+      </c>
+      <c r="K162" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="L162" s="45" t="s">
+        <v>469</v>
+      </c>
+      <c r="M162" s="19"/>
+      <c r="N162" s="12" t="s">
+        <v>424</v>
+      </c>
+      <c r="O162" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="P162" s="12"/>
+      <c r="Q162" s="12"/>
+      <c r="R162" s="12"/>
+      <c r="S162" s="12"/>
+      <c r="T162" s="12"/>
+      <c r="U162" s="12"/>
+      <c r="V162" s="12"/>
+      <c r="W162" s="12">
+        <v>1</v>
+      </c>
+      <c r="X162" s="12"/>
+      <c r="Y162" s="12"/>
+      <c r="Z162" s="12"/>
+      <c r="AA162" s="12"/>
+      <c r="AB162" s="12"/>
+      <c r="AC162" s="12"/>
+      <c r="AD162" s="15">
+        <v>1</v>
+      </c>
+      <c r="AE162" s="44" t="s">
+        <v>77</v>
+      </c>
+      <c r="AF162" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="AG162" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="AH162" s="20">
+        <v>0.1</v>
+      </c>
+      <c r="AI162" s="13">
+        <v>0.15000000000000002</v>
+      </c>
+      <c r="AJ162" s="13">
+        <v>0.1</v>
+      </c>
+      <c r="AK162" s="13">
+        <v>0.15000000000000002</v>
+      </c>
+      <c r="AL162" s="39">
+        <v>6</v>
+      </c>
+      <c r="AM162" s="40">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="163" spans="1:40" ht="140.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A163" s="11" t="s">
+        <v>593</v>
+      </c>
+      <c r="B163" s="12" t="s">
+        <v>594</v>
+      </c>
+      <c r="C163" s="12" t="s">
+        <v>595</v>
+      </c>
+      <c r="D163" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="E163" s="12" t="s">
+        <v>568</v>
+      </c>
+      <c r="F163" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="G163" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="H163" s="12"/>
+      <c r="I163" s="15" t="s">
+        <v>421</v>
+      </c>
+      <c r="J163" s="24" t="s">
+        <v>596</v>
+      </c>
+      <c r="K163" s="12" t="s">
+        <v>235</v>
+      </c>
+      <c r="L163" s="45" t="s">
+        <v>469</v>
+      </c>
+      <c r="M163" s="19"/>
+      <c r="N163" s="12" t="s">
+        <v>424</v>
+      </c>
+      <c r="O163" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="P163" s="12"/>
+      <c r="Q163" s="12"/>
+      <c r="R163" s="12"/>
+      <c r="S163" s="12"/>
+      <c r="T163" s="12"/>
+      <c r="U163" s="12"/>
+      <c r="V163" s="12"/>
+      <c r="W163" s="12"/>
+      <c r="X163" s="12"/>
+      <c r="Y163" s="12"/>
+      <c r="Z163" s="12">
+        <v>1</v>
+      </c>
+      <c r="AA163" s="12"/>
+      <c r="AB163" s="12"/>
+      <c r="AC163" s="12"/>
+      <c r="AD163" s="15">
+        <v>1</v>
+      </c>
+      <c r="AE163" s="44" t="s">
+        <v>77</v>
+      </c>
+      <c r="AF163" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="AG163" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="AH163" s="20">
+        <v>0.1</v>
+      </c>
+      <c r="AI163" s="13">
+        <v>0.15000000000000002</v>
+      </c>
+      <c r="AJ163" s="13">
+        <v>0.1</v>
+      </c>
+      <c r="AK163" s="13">
+        <v>0.15000000000000002</v>
+      </c>
+      <c r="AL163" s="39">
+        <v>6</v>
+      </c>
+      <c r="AM163" s="40">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="164" spans="1:40" ht="140.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A164" s="11" t="s">
+        <v>597</v>
+      </c>
+      <c r="B164" s="12" t="s">
+        <v>598</v>
+      </c>
+      <c r="C164" s="12" t="s">
+        <v>599</v>
+      </c>
+      <c r="D164" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="E164" s="12" t="s">
+        <v>568</v>
+      </c>
+      <c r="F164" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="G164" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="H164" s="12"/>
+      <c r="I164" s="15" t="s">
+        <v>421</v>
+      </c>
+      <c r="J164" s="24" t="s">
+        <v>433</v>
+      </c>
+      <c r="K164" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="L164" s="45" t="s">
+        <v>469</v>
+      </c>
+      <c r="M164" s="19"/>
+      <c r="N164" s="12" t="s">
+        <v>424</v>
+      </c>
+      <c r="O164" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="P164" s="12"/>
+      <c r="Q164" s="12"/>
+      <c r="R164" s="12"/>
+      <c r="S164" s="12"/>
+      <c r="T164" s="12"/>
+      <c r="U164" s="12"/>
+      <c r="V164" s="12"/>
+      <c r="W164" s="12">
+        <v>1</v>
+      </c>
+      <c r="X164" s="12"/>
+      <c r="Y164" s="12"/>
+      <c r="Z164" s="12"/>
+      <c r="AA164" s="12"/>
+      <c r="AB164" s="12"/>
+      <c r="AC164" s="12"/>
+      <c r="AD164" s="15">
+        <v>1</v>
+      </c>
+      <c r="AE164" s="44" t="s">
+        <v>77</v>
+      </c>
+      <c r="AF164" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="AG164" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="AH164" s="20">
+        <v>0.1</v>
+      </c>
+      <c r="AI164" s="13">
+        <v>0.15000000000000002</v>
+      </c>
+      <c r="AJ164" s="13">
+        <v>0.1</v>
+      </c>
+      <c r="AK164" s="13">
+        <v>0.15000000000000002</v>
+      </c>
+      <c r="AL164" s="39">
+        <v>6</v>
+      </c>
+      <c r="AM164" s="40">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="165" spans="1:40" ht="140.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A165" s="11" t="s">
+        <v>600</v>
+      </c>
+      <c r="B165" s="12" t="s">
+        <v>601</v>
+      </c>
+      <c r="C165" s="12" t="s">
+        <v>602</v>
+      </c>
+      <c r="D165" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="E165" s="12" t="s">
+        <v>568</v>
+      </c>
+      <c r="F165" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="G165" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="H165" s="12"/>
+      <c r="I165" s="15" t="s">
+        <v>421</v>
+      </c>
+      <c r="J165" s="24" t="s">
+        <v>603</v>
+      </c>
+      <c r="K165" s="12" t="s">
+        <v>142</v>
+      </c>
+      <c r="L165" s="45" t="s">
+        <v>469</v>
+      </c>
+      <c r="M165" s="19"/>
+      <c r="N165" s="12" t="s">
+        <v>424</v>
+      </c>
+      <c r="O165" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="P165" s="12"/>
+      <c r="Q165" s="12"/>
+      <c r="R165" s="12"/>
+      <c r="S165" s="12"/>
+      <c r="T165" s="12"/>
+      <c r="U165" s="12"/>
+      <c r="V165" s="12"/>
+      <c r="W165" s="12"/>
+      <c r="X165" s="12"/>
+      <c r="Y165" s="12"/>
+      <c r="Z165" s="12">
+        <v>1</v>
+      </c>
+      <c r="AA165" s="12"/>
+      <c r="AB165" s="12"/>
+      <c r="AC165" s="12"/>
+      <c r="AD165" s="15">
+        <v>1</v>
+      </c>
+      <c r="AE165" s="44" t="s">
+        <v>77</v>
+      </c>
+      <c r="AF165" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="AG165" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="AH165" s="20">
+        <v>0.1</v>
+      </c>
+      <c r="AI165" s="13">
+        <v>0.15000000000000002</v>
+      </c>
+      <c r="AJ165" s="13">
+        <v>0.1</v>
+      </c>
+      <c r="AK165" s="13">
+        <v>0.15000000000000002</v>
+      </c>
+      <c r="AL165" s="39">
+        <v>6</v>
+      </c>
+      <c r="AM165" s="40">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="166" spans="1:40" ht="140.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A166" s="11" t="s">
+        <v>604</v>
+      </c>
+      <c r="B166" s="12" t="s">
+        <v>605</v>
+      </c>
+      <c r="C166" s="12" t="s">
+        <v>606</v>
+      </c>
+      <c r="D166" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="E166" s="12" t="s">
+        <v>568</v>
+      </c>
+      <c r="F166" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="G166" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="H166" s="12"/>
+      <c r="I166" s="15" t="s">
+        <v>421</v>
+      </c>
+      <c r="J166" s="24" t="s">
+        <v>607</v>
+      </c>
+      <c r="K166" s="12" t="s">
+        <v>608</v>
+      </c>
+      <c r="L166" s="45" t="s">
+        <v>469</v>
+      </c>
+      <c r="M166" s="19"/>
+      <c r="N166" s="12" t="s">
+        <v>424</v>
+      </c>
+      <c r="O166" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="P166" s="12"/>
+      <c r="Q166" s="12"/>
+      <c r="R166" s="12"/>
+      <c r="S166" s="12"/>
+      <c r="T166" s="12"/>
+      <c r="U166" s="12">
+        <v>1</v>
+      </c>
+      <c r="V166" s="12"/>
+      <c r="W166" s="12"/>
+      <c r="X166" s="12"/>
+      <c r="Y166" s="12"/>
+      <c r="Z166" s="12"/>
+      <c r="AA166" s="12"/>
+      <c r="AB166" s="12"/>
+      <c r="AC166" s="12"/>
+      <c r="AD166" s="15">
+        <v>1</v>
+      </c>
+      <c r="AE166" s="44" t="s">
+        <v>77</v>
+      </c>
+      <c r="AF166" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="AG166" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="AH166" s="20">
+        <v>0.1</v>
+      </c>
+      <c r="AI166" s="13">
+        <v>0.15000000000000002</v>
+      </c>
+      <c r="AJ166" s="13">
+        <v>0.1</v>
+      </c>
+      <c r="AK166" s="13">
+        <v>0.15000000000000002</v>
+      </c>
+      <c r="AL166" s="39">
+        <v>6</v>
+      </c>
+      <c r="AM166" s="40">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="167" spans="1:40" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B167" s="28"/>
+      <c r="D167" s="26"/>
+      <c r="E167" s="23"/>
+      <c r="F167" s="26"/>
+      <c r="G167" s="29"/>
+      <c r="J167" s="32"/>
+      <c r="K167" s="30"/>
+      <c r="L167" s="26"/>
+      <c r="M167" s="41"/>
+      <c r="N167" s="32"/>
+      <c r="AD167" s="26"/>
+      <c r="AE167" s="47"/>
+      <c r="AF167" s="48"/>
+      <c r="AG167" s="29"/>
+      <c r="AH167" s="29"/>
+      <c r="AI167" s="33"/>
+      <c r="AL167" s="23"/>
+      <c r="AM167" s="42"/>
+      <c r="AN167" s="42"/>
+    </row>
+    <row r="168" spans="1:40" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B168" s="28"/>
+      <c r="D168" s="26"/>
+      <c r="E168" s="23"/>
+      <c r="F168" s="26"/>
+      <c r="G168" s="29"/>
+      <c r="J168" s="32"/>
+      <c r="K168" s="30"/>
+      <c r="L168" s="26"/>
+      <c r="M168" s="41"/>
+      <c r="N168" s="32"/>
+      <c r="AD168" s="15">
+        <f>SUM(AD2:AD166)</f>
+        <v>1775</v>
+      </c>
+      <c r="AF168" s="48"/>
+      <c r="AG168" s="29"/>
+      <c r="AH168" s="29"/>
+      <c r="AI168" s="33"/>
+      <c r="AJ168" s="13">
+        <f>SUM(AJ2:AJ166)</f>
+        <v>177.49999999999986</v>
+      </c>
+      <c r="AK168" s="13">
+        <f>SUM(AK2:AK166)</f>
+        <v>266.24999999999881</v>
+      </c>
+      <c r="AM168" s="42"/>
+      <c r="AN168" s="42"/>
+    </row>
+    <row r="169" spans="1:40" ht="140.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="170" spans="1:40" ht="140.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="171" spans="1:40" ht="140.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="172" spans="1:40" ht="140.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="173" spans="1:40" ht="140.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="174" spans="1:40" ht="140.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="175" spans="1:40" ht="140.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="176" spans="1:40" ht="140.1" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="177" ht="140.1" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="178" ht="140.1" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="179" ht="140.1" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -40040,9 +41602,9 @@
   </sheetPr>
   <dimension ref="A1:AM153"/>
   <sheetViews>
-    <sheetView topLeftCell="J1" zoomScale="65" zoomScaleNormal="65" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="P7" sqref="P7"/>
+    <sheetView zoomScale="65" zoomScaleNormal="65" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A13" sqref="A13:AM14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="98.1" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>